<commit_message>
modified predictor, finished base weight function
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>604.13</v>
+        <v>575.9299999999999</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>611.48</v>
+        <v>587.0599999999999</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>572.55</v>
+        <v>557.61</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>605.8099999999999</v>
+        <v>581.3</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>605.8099999999999</v>
+        <v>581.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished applying weight penalty, starting randomsearchcv
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>575.9299999999999</v>
+        <v>601.05</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>587.0599999999999</v>
+        <v>633.8</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>557.61</v>
+        <v>576.42</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>581.3</v>
+        <v>617.08</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>581.3</v>
+        <v>617.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
found best params from randomsearchcv
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>601.05</v>
+        <v>607.22</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>633.8</v>
+        <v>635.0700000000001</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>576.42</v>
+        <v>590.08</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>617.08</v>
+        <v>617.96</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>617.08</v>
+        <v>617.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started candlestick indicator analysis, moving forward with litewick
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>607.22</v>
+        <v>603.8</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>635.0700000000001</v>
+        <v>626.26</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>590.08</v>
+        <v>587.6799999999999</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>617.96</v>
+        <v>614.89</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>617.96</v>
+        <v>614.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created litewick v1, updated predictor to use biaswrappers
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>603.8</v>
+        <v>606.38</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>626.26</v>
+        <v>620.49</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>587.6799999999999</v>
+        <v>602.97</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>614.89</v>
+        <v>620.3</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>614.89</v>
+        <v>620.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started screener, finished turning all patterns to code
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>606.38</v>
+        <v>604.86</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>620.49</v>
+        <v>597.38</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>602.97</v>
+        <v>585.78</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>620.3</v>
+        <v>586.49</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>620.3</v>
+        <v>586.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created screener.py, about to start experimenting with splitting datasets into O-H-L-C-AC
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>604.86</v>
+        <v>618.8099999999999</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>597.38</v>
+        <v>643.89</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>585.78</v>
+        <v>612.58</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>586.49</v>
+        <v>628.23</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>586.49</v>
+        <v>628.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified litewick for optim, working on more-than-one-day sentiment analysis with weighter
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>618.8099999999999</v>
+        <v>678.21</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>643.89</v>
+        <v>685.6799999999999</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>612.58</v>
+        <v>670.89</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>628.23</v>
+        <v>667.78</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>628.23</v>
+        <v>667.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished 8ball gen 1!!! building the great botsicle
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>678.21</v>
+        <v>591.15</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>685.6799999999999</v>
+        <v>612.04</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>670.89</v>
+        <v>579.0599999999999</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>667.78</v>
+        <v>609.99</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>667.78</v>
+        <v>609.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actually finished gen 1, completed with basic sentiment analysis. starting testtrade now!
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>591.15</v>
+        <v>657.09</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>612.04</v>
+        <v>674.85</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>579.0599999999999</v>
+        <v>647.0700000000001</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>609.99</v>
+        <v>657.64</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>609.99</v>
+        <v>657.64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished tweet alternatives, going to improve news and clean code and stuff things in archive
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>657.09</v>
+        <v>701.09</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>674.85</v>
+        <v>724.25</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>647.0700000000001</v>
+        <v>700.77</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>657.64</v>
+        <v>719.63</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>657.64</v>
+        <v>719.63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
for real FINALLY FINISHED MULTIPROCESSING now tweaking models and params
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>736.22</v>
+        <v>1046.57</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>740.77</v>
+        <v>1073.18</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>713.71</v>
+        <v>1022.86</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>710.33</v>
+        <v>1061.48</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>710.33</v>
+        <v>1061.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving all work so I can try RAPIDS
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1046.57</v>
+        <v>830.04</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1073.18</v>
+        <v>841.34</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1022.86</v>
+        <v>807.87</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1061.48</v>
+        <v>813.52</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1061.48</v>
+        <v>813.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
returning to this after a year or so...let's see if we can make this work
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>830.04</v>
+        <v>1070.53</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>841.34</v>
+        <v>1072.12</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>807.87</v>
+        <v>1012.18</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>813.52</v>
+        <v>1019.23</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>813.52</v>
+        <v>1019.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>